<commit_message>
Vault backup: 26/04/24 10:31:39 XMG
Affected files:
.obsidian/workspace.json
A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
Backlog_0424.md
ITP/Theorie/Klassenliste.xlsx
</commit_message>
<xml_diff>
--- a/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
+++ b/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\2023_24_4BHITS\A_Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C7B427-717E-4A83-A350-6D516D6BEA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE9133-5430-4704-972F-1E21979533BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Name:</t>
   </si>
@@ -193,6 +193,9 @@
   <si>
     <t>Poster designen, Testdruck</t>
   </si>
+  <si>
+    <t>STRG + .</t>
+  </si>
 </sst>
 </file>
 
@@ -270,7 +273,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +302,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
         <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -685,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -863,6 +872,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1985,7 +1997,7 @@
   <dimension ref="A1:HZ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2435,6 +2447,9 @@
         <v>0</v>
       </c>
       <c r="H9" s="16"/>
+      <c r="J9" s="61" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
@@ -6880,7 +6895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
@@ -7393,9 +7408,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7543,25 +7561,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7585,9 +7593,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Vault backup: 03/05/24 13:06:44 XMG
Affected files:
.obsidian/workspace.json
AM/binomialverteilung_aufgaben.pdf
A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
Backlog_0524.md
DE/Kommentar Q&A.md
DE/Kommentar Q&A.pdf
ITP/Theorie/K5_LE2_EVA.xlsx
</commit_message>
<xml_diff>
--- a/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
+++ b/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\2023_24_4BHITS\A_Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE9133-5430-4704-972F-1E21979533BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C691244-39D6-40BB-A150-0A75667387F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Begleitprotokoll" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Begleitprotokoll!$A$1:$H$33</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Name:</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Arbeitszeit:</t>
   </si>
   <si>
-    <t>Vorname Nachname</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erste Besprechung, Erste Besprechung in Eggenburg </t>
   </si>
   <si>
@@ -195,6 +192,12 @@
   </si>
   <si>
     <t>STRG + .</t>
+  </si>
+  <si>
+    <t>Besprechung weiteres Vorgehen, Inhalt, Technisches, Themenbereich besprochen</t>
+  </si>
+  <si>
+    <t>Matthias Hrbek</t>
   </si>
 </sst>
 </file>
@@ -775,7 +778,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -810,6 +812,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -872,9 +878,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1245,7 +1248,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.4166666666666665</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1997,7 +2000,7 @@
   <dimension ref="A1:HZ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,61 +2016,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="24">
         <f>SUM(E5:E209)</f>
-        <v>0.83</v>
+        <v>4.25</v>
       </c>
       <c r="F2" s="24">
         <f>SUM(F5:F209)</f>
-        <v>5.836666666666666</v>
+        <v>5.8333333333333321</v>
       </c>
       <c r="G2" s="25">
         <f>SUM(G5:G209)</f>
-        <v>6.6666666666666661</v>
+        <v>10.083333333333332</v>
       </c>
       <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:234" s="8" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="49" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="7"/>
@@ -2298,18 +2301,18 @@
       <c r="HZ3" s="7"/>
     </row>
     <row r="4" spans="1:234" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="28" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="49"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="50"/>
     </row>
     <row r="5" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
@@ -2325,19 +2328,19 @@
       <c r="D5" s="13">
         <v>0.65277777777777779</v>
       </c>
-      <c r="E5" s="29">
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
+      <c r="E5" s="28">
+        <v>0</v>
+      </c>
+      <c r="F5" s="29">
         <f>G5-E5</f>
         <v>2.1666666666666665</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <f t="shared" ref="G5:G72" si="1">HOUR($D5-$C5)+MINUTE($D5-$C5)/60</f>
         <v>2.1666666666666665</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:234" x14ac:dyDescent="0.3">
@@ -2354,19 +2357,19 @@
       <c r="D6" s="13">
         <v>0.90277777777777779</v>
       </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
+      <c r="E6" s="29">
+        <v>0</v>
+      </c>
+      <c r="F6" s="29">
         <f t="shared" ref="F6:F73" si="2">G6-E6</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <f t="shared" si="1"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:234" x14ac:dyDescent="0.3">
@@ -2383,19 +2386,19 @@
       <c r="D7" s="13">
         <v>0.54861111111111116</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>0.83</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <f t="shared" si="2"/>
         <v>3.3333333333334103E-3</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:234" x14ac:dyDescent="0.3">
@@ -2412,43 +2415,51 @@
       <c r="D8" s="13">
         <v>0.6875</v>
       </c>
-      <c r="E8" s="30">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="29">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="H8" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:234" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>45414</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E9" s="29">
+        <v>3.42</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="2"/>
+        <v>-3.3333333333334103E-3</v>
+      </c>
+      <c r="G9" s="28">
+        <f t="shared" si="1"/>
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:234" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="11" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="30">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="J9" s="61" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:234" x14ac:dyDescent="0.3">
@@ -2459,14 +2470,14 @@
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="30">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2480,14 +2491,14 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="30">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30">
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2501,14 +2512,14 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="30">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30">
+      <c r="E12" s="29">
+        <v>0</v>
+      </c>
+      <c r="F12" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2522,14 +2533,14 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="30">
-        <v>0</v>
-      </c>
-      <c r="F13" s="30">
+      <c r="E13" s="29">
+        <v>0</v>
+      </c>
+      <c r="F13" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2543,14 +2554,14 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="30">
-        <v>0</v>
-      </c>
-      <c r="F14" s="30">
+      <c r="E14" s="29">
+        <v>0</v>
+      </c>
+      <c r="F14" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2564,14 +2575,14 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="30">
-        <v>0</v>
-      </c>
-      <c r="F15" s="30">
+      <c r="E15" s="29">
+        <v>0</v>
+      </c>
+      <c r="F15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2585,14 +2596,14 @@
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="30">
-        <v>0</v>
-      </c>
-      <c r="F16" s="30">
+      <c r="E16" s="29">
+        <v>0</v>
+      </c>
+      <c r="F16" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2606,14 +2617,14 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="30">
-        <v>0</v>
-      </c>
-      <c r="F17" s="30">
+      <c r="E17" s="29">
+        <v>0</v>
+      </c>
+      <c r="F17" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2627,14 +2638,14 @@
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="30">
-        <v>0</v>
-      </c>
-      <c r="F18" s="30">
+      <c r="E18" s="29">
+        <v>0</v>
+      </c>
+      <c r="F18" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2648,18 +2659,18 @@
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="30">
-        <v>0</v>
-      </c>
-      <c r="F19" s="30">
+      <c r="E19" s="29">
+        <v>0</v>
+      </c>
+      <c r="F19" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="27"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
@@ -2669,14 +2680,14 @@
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="30">
-        <v>0</v>
-      </c>
-      <c r="F20" s="30">
+      <c r="E20" s="29">
+        <v>0</v>
+      </c>
+      <c r="F20" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2690,14 +2701,14 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="30">
-        <v>0</v>
-      </c>
-      <c r="F21" s="30">
+      <c r="E21" s="29">
+        <v>0</v>
+      </c>
+      <c r="F21" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2711,14 +2722,14 @@
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="30">
-        <v>0</v>
-      </c>
-      <c r="F22" s="30">
+      <c r="E22" s="29">
+        <v>0</v>
+      </c>
+      <c r="F22" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2732,14 +2743,14 @@
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="30">
-        <v>0</v>
-      </c>
-      <c r="F23" s="30">
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2753,14 +2764,14 @@
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="30">
-        <v>0</v>
-      </c>
-      <c r="F24" s="30">
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
+      <c r="F24" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2774,14 +2785,14 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="30">
-        <v>0</v>
-      </c>
-      <c r="F25" s="30">
+      <c r="E25" s="29">
+        <v>0</v>
+      </c>
+      <c r="F25" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2795,14 +2806,14 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="30">
-        <v>0</v>
-      </c>
-      <c r="F26" s="30">
+      <c r="E26" s="29">
+        <v>0</v>
+      </c>
+      <c r="F26" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2816,14 +2827,14 @@
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="30">
-        <v>0</v>
-      </c>
-      <c r="F27" s="30">
+      <c r="E27" s="29">
+        <v>0</v>
+      </c>
+      <c r="F27" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2837,14 +2848,14 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="30">
-        <v>0</v>
-      </c>
-      <c r="F28" s="30">
+      <c r="E28" s="29">
+        <v>0</v>
+      </c>
+      <c r="F28" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2858,14 +2869,14 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="30">
-        <v>0</v>
-      </c>
-      <c r="F29" s="30">
+      <c r="E29" s="29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2879,14 +2890,14 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="30">
-        <v>0</v>
-      </c>
-      <c r="F30" s="30">
+      <c r="E30" s="29">
+        <v>0</v>
+      </c>
+      <c r="F30" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2900,14 +2911,14 @@
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="30">
-        <v>0</v>
-      </c>
-      <c r="F31" s="30">
+      <c r="E31" s="29">
+        <v>0</v>
+      </c>
+      <c r="F31" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2921,14 +2932,14 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="30">
-        <v>0</v>
-      </c>
-      <c r="F32" s="30">
+      <c r="E32" s="29">
+        <v>0</v>
+      </c>
+      <c r="F32" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G32" s="29">
+      <c r="G32" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2942,14 +2953,14 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="13"/>
-      <c r="E33" s="30">
-        <v>0</v>
-      </c>
-      <c r="F33" s="30">
+      <c r="E33" s="29">
+        <v>0</v>
+      </c>
+      <c r="F33" s="29">
         <f t="shared" ref="F33" si="4">G33-E33</f>
         <v>0</v>
       </c>
-      <c r="G33" s="29">
+      <c r="G33" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2963,14 +2974,14 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="30">
-        <v>0</v>
-      </c>
-      <c r="F34" s="30">
+      <c r="E34" s="29">
+        <v>0</v>
+      </c>
+      <c r="F34" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2984,14 +2995,14 @@
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="30">
-        <v>0</v>
-      </c>
-      <c r="F35" s="30">
+      <c r="E35" s="29">
+        <v>0</v>
+      </c>
+      <c r="F35" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G35" s="29">
+      <c r="G35" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3005,14 +3016,14 @@
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
-      <c r="E36" s="30">
-        <v>0</v>
-      </c>
-      <c r="F36" s="30">
+      <c r="E36" s="29">
+        <v>0</v>
+      </c>
+      <c r="F36" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3026,14 +3037,14 @@
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="30">
-        <v>0</v>
-      </c>
-      <c r="F37" s="30">
+      <c r="E37" s="29">
+        <v>0</v>
+      </c>
+      <c r="F37" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="29">
+      <c r="G37" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3047,14 +3058,14 @@
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="30">
-        <v>0</v>
-      </c>
-      <c r="F38" s="30">
+      <c r="E38" s="29">
+        <v>0</v>
+      </c>
+      <c r="F38" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3068,14 +3079,14 @@
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="30">
-        <v>0</v>
-      </c>
-      <c r="F39" s="30">
+      <c r="E39" s="29">
+        <v>0</v>
+      </c>
+      <c r="F39" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3089,14 +3100,14 @@
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="30">
-        <v>0</v>
-      </c>
-      <c r="F40" s="30">
+      <c r="E40" s="29">
+        <v>0</v>
+      </c>
+      <c r="F40" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3110,14 +3121,14 @@
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
-      <c r="E41" s="30">
-        <v>0</v>
-      </c>
-      <c r="F41" s="30">
+      <c r="E41" s="29">
+        <v>0</v>
+      </c>
+      <c r="F41" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G41" s="29">
+      <c r="G41" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3131,14 +3142,14 @@
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="30">
-        <v>0</v>
-      </c>
-      <c r="F42" s="30">
+      <c r="E42" s="29">
+        <v>0</v>
+      </c>
+      <c r="F42" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3152,14 +3163,14 @@
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="13"/>
-      <c r="E43" s="30">
-        <v>0</v>
-      </c>
-      <c r="F43" s="30">
+      <c r="E43" s="29">
+        <v>0</v>
+      </c>
+      <c r="F43" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G43" s="29">
+      <c r="G43" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3173,14 +3184,14 @@
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="13"/>
-      <c r="E44" s="30">
-        <v>0</v>
-      </c>
-      <c r="F44" s="30">
+      <c r="E44" s="29">
+        <v>0</v>
+      </c>
+      <c r="F44" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G44" s="29">
+      <c r="G44" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3194,14 +3205,14 @@
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="30">
-        <v>0</v>
-      </c>
-      <c r="F45" s="30">
+      <c r="E45" s="29">
+        <v>0</v>
+      </c>
+      <c r="F45" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3215,14 +3226,14 @@
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="30">
-        <v>0</v>
-      </c>
-      <c r="F46" s="30">
+      <c r="E46" s="29">
+        <v>0</v>
+      </c>
+      <c r="F46" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G46" s="29">
+      <c r="G46" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3236,14 +3247,14 @@
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="30">
-        <v>0</v>
-      </c>
-      <c r="F47" s="30">
+      <c r="E47" s="29">
+        <v>0</v>
+      </c>
+      <c r="F47" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G47" s="29">
+      <c r="G47" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3257,14 +3268,14 @@
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="30">
-        <v>0</v>
-      </c>
-      <c r="F48" s="30">
+      <c r="E48" s="29">
+        <v>0</v>
+      </c>
+      <c r="F48" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G48" s="29">
+      <c r="G48" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3278,14 +3289,14 @@
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="30">
-        <v>0</v>
-      </c>
-      <c r="F49" s="30">
+      <c r="E49" s="29">
+        <v>0</v>
+      </c>
+      <c r="F49" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G49" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3299,14 +3310,14 @@
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="30">
-        <v>0</v>
-      </c>
-      <c r="F50" s="30">
+      <c r="E50" s="29">
+        <v>0</v>
+      </c>
+      <c r="F50" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G50" s="29">
+      <c r="G50" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3320,14 +3331,14 @@
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="30">
-        <v>0</v>
-      </c>
-      <c r="F51" s="30">
+      <c r="E51" s="29">
+        <v>0</v>
+      </c>
+      <c r="F51" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G51" s="29">
+      <c r="G51" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3341,14 +3352,14 @@
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="30">
-        <v>0</v>
-      </c>
-      <c r="F52" s="30">
+      <c r="E52" s="29">
+        <v>0</v>
+      </c>
+      <c r="F52" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G52" s="29">
+      <c r="G52" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3362,14 +3373,14 @@
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="30">
-        <v>0</v>
-      </c>
-      <c r="F53" s="30">
+      <c r="E53" s="29">
+        <v>0</v>
+      </c>
+      <c r="F53" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G53" s="29">
+      <c r="G53" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3383,14 +3394,14 @@
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="13"/>
-      <c r="E54" s="30">
-        <v>0</v>
-      </c>
-      <c r="F54" s="30">
+      <c r="E54" s="29">
+        <v>0</v>
+      </c>
+      <c r="F54" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G54" s="29">
+      <c r="G54" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3404,14 +3415,14 @@
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="13"/>
-      <c r="E55" s="30">
-        <v>0</v>
-      </c>
-      <c r="F55" s="30">
+      <c r="E55" s="29">
+        <v>0</v>
+      </c>
+      <c r="F55" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G55" s="29">
+      <c r="G55" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3425,14 +3436,14 @@
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="30">
-        <v>0</v>
-      </c>
-      <c r="F56" s="30">
+      <c r="E56" s="29">
+        <v>0</v>
+      </c>
+      <c r="F56" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G56" s="29">
+      <c r="G56" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3446,14 +3457,14 @@
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="13"/>
-      <c r="E57" s="30">
-        <v>0</v>
-      </c>
-      <c r="F57" s="30">
+      <c r="E57" s="29">
+        <v>0</v>
+      </c>
+      <c r="F57" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G57" s="29">
+      <c r="G57" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3467,14 +3478,14 @@
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="30">
-        <v>0</v>
-      </c>
-      <c r="F58" s="30">
+      <c r="E58" s="29">
+        <v>0</v>
+      </c>
+      <c r="F58" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G58" s="29">
+      <c r="G58" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3488,14 +3499,14 @@
       </c>
       <c r="C59" s="12"/>
       <c r="D59" s="13"/>
-      <c r="E59" s="30">
-        <v>0</v>
-      </c>
-      <c r="F59" s="30">
+      <c r="E59" s="29">
+        <v>0</v>
+      </c>
+      <c r="F59" s="29">
         <f t="shared" ref="F59" si="6">G59-E59</f>
         <v>0</v>
       </c>
-      <c r="G59" s="29">
+      <c r="G59" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3509,14 +3520,14 @@
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="30">
-        <v>0</v>
-      </c>
-      <c r="F60" s="30">
+      <c r="E60" s="29">
+        <v>0</v>
+      </c>
+      <c r="F60" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G60" s="29">
+      <c r="G60" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3530,14 +3541,14 @@
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="13"/>
-      <c r="E61" s="30">
-        <v>0</v>
-      </c>
-      <c r="F61" s="30">
+      <c r="E61" s="29">
+        <v>0</v>
+      </c>
+      <c r="F61" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G61" s="29">
+      <c r="G61" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3551,14 +3562,14 @@
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="30">
-        <v>0</v>
-      </c>
-      <c r="F62" s="30">
+      <c r="E62" s="29">
+        <v>0</v>
+      </c>
+      <c r="F62" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G62" s="29">
+      <c r="G62" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3572,14 +3583,14 @@
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="30">
-        <v>0</v>
-      </c>
-      <c r="F63" s="30">
+      <c r="E63" s="29">
+        <v>0</v>
+      </c>
+      <c r="F63" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G63" s="29">
+      <c r="G63" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3593,14 +3604,14 @@
       </c>
       <c r="C64" s="12"/>
       <c r="D64" s="13"/>
-      <c r="E64" s="30">
-        <v>0</v>
-      </c>
-      <c r="F64" s="30">
+      <c r="E64" s="29">
+        <v>0</v>
+      </c>
+      <c r="F64" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G64" s="29">
+      <c r="G64" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3614,14 +3625,14 @@
       </c>
       <c r="C65" s="12"/>
       <c r="D65" s="13"/>
-      <c r="E65" s="30">
-        <v>0</v>
-      </c>
-      <c r="F65" s="30">
+      <c r="E65" s="29">
+        <v>0</v>
+      </c>
+      <c r="F65" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G65" s="29">
+      <c r="G65" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3635,14 +3646,14 @@
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="13"/>
-      <c r="E66" s="30">
-        <v>0</v>
-      </c>
-      <c r="F66" s="30">
+      <c r="E66" s="29">
+        <v>0</v>
+      </c>
+      <c r="F66" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G66" s="29">
+      <c r="G66" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3656,14 +3667,14 @@
       </c>
       <c r="C67" s="12"/>
       <c r="D67" s="13"/>
-      <c r="E67" s="30">
-        <v>0</v>
-      </c>
-      <c r="F67" s="30">
+      <c r="E67" s="29">
+        <v>0</v>
+      </c>
+      <c r="F67" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G67" s="29">
+      <c r="G67" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3677,14 +3688,14 @@
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="13"/>
-      <c r="E68" s="30">
-        <v>0</v>
-      </c>
-      <c r="F68" s="30">
+      <c r="E68" s="29">
+        <v>0</v>
+      </c>
+      <c r="F68" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G68" s="29">
+      <c r="G68" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3698,14 +3709,14 @@
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="13"/>
-      <c r="E69" s="30">
-        <v>0</v>
-      </c>
-      <c r="F69" s="30">
+      <c r="E69" s="29">
+        <v>0</v>
+      </c>
+      <c r="F69" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G69" s="29">
+      <c r="G69" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3719,14 +3730,14 @@
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="13"/>
-      <c r="E70" s="30">
-        <v>0</v>
-      </c>
-      <c r="F70" s="30">
+      <c r="E70" s="29">
+        <v>0</v>
+      </c>
+      <c r="F70" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G70" s="29">
+      <c r="G70" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3740,14 +3751,14 @@
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="13"/>
-      <c r="E71" s="30">
-        <v>0</v>
-      </c>
-      <c r="F71" s="30">
+      <c r="E71" s="29">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G71" s="29">
+      <c r="G71" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3761,14 +3772,14 @@
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="30">
-        <v>0</v>
-      </c>
-      <c r="F72" s="30">
+      <c r="E72" s="29">
+        <v>0</v>
+      </c>
+      <c r="F72" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G72" s="29">
+      <c r="G72" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3782,14 +3793,14 @@
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="30">
-        <v>0</v>
-      </c>
-      <c r="F73" s="30">
+      <c r="E73" s="29">
+        <v>0</v>
+      </c>
+      <c r="F73" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G73" s="29">
+      <c r="G73" s="28">
         <f t="shared" ref="G73:G139" si="7">HOUR($D73-$C73)+MINUTE($D73-$C73)/60</f>
         <v>0</v>
       </c>
@@ -3803,14 +3814,14 @@
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="13"/>
-      <c r="E74" s="30">
-        <v>0</v>
-      </c>
-      <c r="F74" s="30">
+      <c r="E74" s="29">
+        <v>0</v>
+      </c>
+      <c r="F74" s="29">
         <f>G74-E74</f>
         <v>0</v>
       </c>
-      <c r="G74" s="29">
+      <c r="G74" s="28">
         <f>HOUR($D74-$C74)+MINUTE($D74-$C74)/60</f>
         <v>0</v>
       </c>
@@ -3824,14 +3835,14 @@
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="30">
-        <v>0</v>
-      </c>
-      <c r="F75" s="30">
+      <c r="E75" s="29">
+        <v>0</v>
+      </c>
+      <c r="F75" s="29">
         <f t="shared" ref="F75:F140" si="9">G75-E75</f>
         <v>0</v>
       </c>
-      <c r="G75" s="29">
+      <c r="G75" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3845,14 +3856,14 @@
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="13"/>
-      <c r="E76" s="30">
-        <v>0</v>
-      </c>
-      <c r="F76" s="30">
+      <c r="E76" s="29">
+        <v>0</v>
+      </c>
+      <c r="F76" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G76" s="29">
+      <c r="G76" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3866,14 +3877,14 @@
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="13"/>
-      <c r="E77" s="30">
-        <v>0</v>
-      </c>
-      <c r="F77" s="30">
+      <c r="E77" s="29">
+        <v>0</v>
+      </c>
+      <c r="F77" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G77" s="29">
+      <c r="G77" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3887,14 +3898,14 @@
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="13"/>
-      <c r="E78" s="30">
-        <v>0</v>
-      </c>
-      <c r="F78" s="30">
+      <c r="E78" s="29">
+        <v>0</v>
+      </c>
+      <c r="F78" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G78" s="29">
+      <c r="G78" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3908,14 +3919,14 @@
       </c>
       <c r="C79" s="12"/>
       <c r="D79" s="13"/>
-      <c r="E79" s="30">
-        <v>0</v>
-      </c>
-      <c r="F79" s="30">
+      <c r="E79" s="29">
+        <v>0</v>
+      </c>
+      <c r="F79" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G79" s="29">
+      <c r="G79" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3929,14 +3940,14 @@
       </c>
       <c r="C80" s="12"/>
       <c r="D80" s="13"/>
-      <c r="E80" s="30">
-        <v>0</v>
-      </c>
-      <c r="F80" s="30">
+      <c r="E80" s="29">
+        <v>0</v>
+      </c>
+      <c r="F80" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G80" s="29">
+      <c r="G80" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3950,14 +3961,14 @@
       </c>
       <c r="C81" s="12"/>
       <c r="D81" s="13"/>
-      <c r="E81" s="30">
-        <v>0</v>
-      </c>
-      <c r="F81" s="30">
+      <c r="E81" s="29">
+        <v>0</v>
+      </c>
+      <c r="F81" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G81" s="29">
+      <c r="G81" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3971,14 +3982,14 @@
       </c>
       <c r="C82" s="12"/>
       <c r="D82" s="13"/>
-      <c r="E82" s="30">
-        <v>0</v>
-      </c>
-      <c r="F82" s="30">
+      <c r="E82" s="29">
+        <v>0</v>
+      </c>
+      <c r="F82" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G82" s="29">
+      <c r="G82" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3992,14 +4003,14 @@
       </c>
       <c r="C83" s="12"/>
       <c r="D83" s="13"/>
-      <c r="E83" s="30">
-        <v>0</v>
-      </c>
-      <c r="F83" s="30">
+      <c r="E83" s="29">
+        <v>0</v>
+      </c>
+      <c r="F83" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G83" s="29">
+      <c r="G83" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4013,14 +4024,14 @@
       </c>
       <c r="C84" s="12"/>
       <c r="D84" s="13"/>
-      <c r="E84" s="30">
-        <v>0</v>
-      </c>
-      <c r="F84" s="30">
+      <c r="E84" s="29">
+        <v>0</v>
+      </c>
+      <c r="F84" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G84" s="29">
+      <c r="G84" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4034,14 +4045,14 @@
       </c>
       <c r="C85" s="12"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="30">
-        <v>0</v>
-      </c>
-      <c r="F85" s="30">
+      <c r="E85" s="29">
+        <v>0</v>
+      </c>
+      <c r="F85" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G85" s="29">
+      <c r="G85" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4055,14 +4066,14 @@
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="13"/>
-      <c r="E86" s="30">
-        <v>0</v>
-      </c>
-      <c r="F86" s="30">
+      <c r="E86" s="29">
+        <v>0</v>
+      </c>
+      <c r="F86" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G86" s="29">
+      <c r="G86" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4076,14 +4087,14 @@
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="13"/>
-      <c r="E87" s="30">
-        <v>0</v>
-      </c>
-      <c r="F87" s="30">
+      <c r="E87" s="29">
+        <v>0</v>
+      </c>
+      <c r="F87" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G87" s="29">
+      <c r="G87" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4097,14 +4108,14 @@
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="13"/>
-      <c r="E88" s="30">
-        <v>0</v>
-      </c>
-      <c r="F88" s="30">
+      <c r="E88" s="29">
+        <v>0</v>
+      </c>
+      <c r="F88" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G88" s="29">
+      <c r="G88" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4118,14 +4129,14 @@
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="13"/>
-      <c r="E89" s="30">
-        <v>0</v>
-      </c>
-      <c r="F89" s="30">
+      <c r="E89" s="29">
+        <v>0</v>
+      </c>
+      <c r="F89" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G89" s="29">
+      <c r="G89" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4139,14 +4150,14 @@
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="13"/>
-      <c r="E90" s="30">
-        <v>0</v>
-      </c>
-      <c r="F90" s="30">
+      <c r="E90" s="29">
+        <v>0</v>
+      </c>
+      <c r="F90" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G90" s="29">
+      <c r="G90" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4160,14 +4171,14 @@
       </c>
       <c r="C91" s="12"/>
       <c r="D91" s="13"/>
-      <c r="E91" s="30">
-        <v>0</v>
-      </c>
-      <c r="F91" s="30">
+      <c r="E91" s="29">
+        <v>0</v>
+      </c>
+      <c r="F91" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G91" s="29">
+      <c r="G91" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4181,14 +4192,14 @@
       </c>
       <c r="C92" s="12"/>
       <c r="D92" s="13"/>
-      <c r="E92" s="30">
-        <v>0</v>
-      </c>
-      <c r="F92" s="30">
+      <c r="E92" s="29">
+        <v>0</v>
+      </c>
+      <c r="F92" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G92" s="29">
+      <c r="G92" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4202,14 +4213,14 @@
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="13"/>
-      <c r="E93" s="30">
-        <v>0</v>
-      </c>
-      <c r="F93" s="30">
+      <c r="E93" s="29">
+        <v>0</v>
+      </c>
+      <c r="F93" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G93" s="29">
+      <c r="G93" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4223,14 +4234,14 @@
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="13"/>
-      <c r="E94" s="30">
-        <v>0</v>
-      </c>
-      <c r="F94" s="30">
+      <c r="E94" s="29">
+        <v>0</v>
+      </c>
+      <c r="F94" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G94" s="29">
+      <c r="G94" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4244,14 +4255,14 @@
       </c>
       <c r="C95" s="12"/>
       <c r="D95" s="13"/>
-      <c r="E95" s="30">
-        <v>0</v>
-      </c>
-      <c r="F95" s="30">
+      <c r="E95" s="29">
+        <v>0</v>
+      </c>
+      <c r="F95" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G95" s="29">
+      <c r="G95" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4265,14 +4276,14 @@
       </c>
       <c r="C96" s="12"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="30">
-        <v>0</v>
-      </c>
-      <c r="F96" s="30">
+      <c r="E96" s="29">
+        <v>0</v>
+      </c>
+      <c r="F96" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G96" s="29">
+      <c r="G96" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4286,14 +4297,14 @@
       </c>
       <c r="C97" s="12"/>
       <c r="D97" s="13"/>
-      <c r="E97" s="30">
-        <v>0</v>
-      </c>
-      <c r="F97" s="30">
+      <c r="E97" s="29">
+        <v>0</v>
+      </c>
+      <c r="F97" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G97" s="29">
+      <c r="G97" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4307,14 +4318,14 @@
       </c>
       <c r="C98" s="12"/>
       <c r="D98" s="13"/>
-      <c r="E98" s="30">
-        <v>0</v>
-      </c>
-      <c r="F98" s="30">
+      <c r="E98" s="29">
+        <v>0</v>
+      </c>
+      <c r="F98" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G98" s="29">
+      <c r="G98" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4328,14 +4339,14 @@
       </c>
       <c r="C99" s="12"/>
       <c r="D99" s="13"/>
-      <c r="E99" s="30">
-        <v>0</v>
-      </c>
-      <c r="F99" s="30">
+      <c r="E99" s="29">
+        <v>0</v>
+      </c>
+      <c r="F99" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G99" s="29">
+      <c r="G99" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4349,14 +4360,14 @@
       </c>
       <c r="C100" s="12"/>
       <c r="D100" s="13"/>
-      <c r="E100" s="30">
-        <v>0</v>
-      </c>
-      <c r="F100" s="30">
+      <c r="E100" s="29">
+        <v>0</v>
+      </c>
+      <c r="F100" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G100" s="29">
+      <c r="G100" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4370,14 +4381,14 @@
       </c>
       <c r="C101" s="12"/>
       <c r="D101" s="13"/>
-      <c r="E101" s="30">
-        <v>0</v>
-      </c>
-      <c r="F101" s="30">
+      <c r="E101" s="29">
+        <v>0</v>
+      </c>
+      <c r="F101" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G101" s="29">
+      <c r="G101" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4391,14 +4402,14 @@
       </c>
       <c r="C102" s="12"/>
       <c r="D102" s="13"/>
-      <c r="E102" s="30">
-        <v>0</v>
-      </c>
-      <c r="F102" s="30">
+      <c r="E102" s="29">
+        <v>0</v>
+      </c>
+      <c r="F102" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G102" s="29">
+      <c r="G102" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4412,14 +4423,14 @@
       </c>
       <c r="C103" s="12"/>
       <c r="D103" s="13"/>
-      <c r="E103" s="30">
-        <v>0</v>
-      </c>
-      <c r="F103" s="30">
+      <c r="E103" s="29">
+        <v>0</v>
+      </c>
+      <c r="F103" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G103" s="29">
+      <c r="G103" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4433,14 +4444,14 @@
       </c>
       <c r="C104" s="12"/>
       <c r="D104" s="13"/>
-      <c r="E104" s="30">
-        <v>0</v>
-      </c>
-      <c r="F104" s="30">
+      <c r="E104" s="29">
+        <v>0</v>
+      </c>
+      <c r="F104" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G104" s="29">
+      <c r="G104" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4454,14 +4465,14 @@
       </c>
       <c r="C105" s="12"/>
       <c r="D105" s="13"/>
-      <c r="E105" s="30">
-        <v>0</v>
-      </c>
-      <c r="F105" s="30">
+      <c r="E105" s="29">
+        <v>0</v>
+      </c>
+      <c r="F105" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G105" s="29">
+      <c r="G105" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4475,14 +4486,14 @@
       </c>
       <c r="C106" s="12"/>
       <c r="D106" s="13"/>
-      <c r="E106" s="30">
-        <v>0</v>
-      </c>
-      <c r="F106" s="30">
+      <c r="E106" s="29">
+        <v>0</v>
+      </c>
+      <c r="F106" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G106" s="29">
+      <c r="G106" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4496,14 +4507,14 @@
       </c>
       <c r="C107" s="12"/>
       <c r="D107" s="13"/>
-      <c r="E107" s="30">
-        <v>0</v>
-      </c>
-      <c r="F107" s="30">
+      <c r="E107" s="29">
+        <v>0</v>
+      </c>
+      <c r="F107" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G107" s="29">
+      <c r="G107" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4517,14 +4528,14 @@
       </c>
       <c r="C108" s="12"/>
       <c r="D108" s="13"/>
-      <c r="E108" s="30">
-        <v>0</v>
-      </c>
-      <c r="F108" s="30">
+      <c r="E108" s="29">
+        <v>0</v>
+      </c>
+      <c r="F108" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G108" s="29">
+      <c r="G108" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4538,14 +4549,14 @@
       </c>
       <c r="C109" s="12"/>
       <c r="D109" s="13"/>
-      <c r="E109" s="30">
-        <v>0</v>
-      </c>
-      <c r="F109" s="30">
+      <c r="E109" s="29">
+        <v>0</v>
+      </c>
+      <c r="F109" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G109" s="29">
+      <c r="G109" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4559,14 +4570,14 @@
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="13"/>
-      <c r="E110" s="30">
-        <v>0</v>
-      </c>
-      <c r="F110" s="30">
+      <c r="E110" s="29">
+        <v>0</v>
+      </c>
+      <c r="F110" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G110" s="29">
+      <c r="G110" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4580,14 +4591,14 @@
       </c>
       <c r="C111" s="12"/>
       <c r="D111" s="13"/>
-      <c r="E111" s="30">
-        <v>0</v>
-      </c>
-      <c r="F111" s="30">
+      <c r="E111" s="29">
+        <v>0</v>
+      </c>
+      <c r="F111" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G111" s="29">
+      <c r="G111" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4601,14 +4612,14 @@
       </c>
       <c r="C112" s="12"/>
       <c r="D112" s="13"/>
-      <c r="E112" s="30">
-        <v>0</v>
-      </c>
-      <c r="F112" s="30">
+      <c r="E112" s="29">
+        <v>0</v>
+      </c>
+      <c r="F112" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G112" s="29">
+      <c r="G112" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4622,14 +4633,14 @@
       </c>
       <c r="C113" s="12"/>
       <c r="D113" s="13"/>
-      <c r="E113" s="30">
-        <v>0</v>
-      </c>
-      <c r="F113" s="30">
+      <c r="E113" s="29">
+        <v>0</v>
+      </c>
+      <c r="F113" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G113" s="29">
+      <c r="G113" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4643,14 +4654,14 @@
       </c>
       <c r="C114" s="12"/>
       <c r="D114" s="13"/>
-      <c r="E114" s="30">
-        <v>0</v>
-      </c>
-      <c r="F114" s="30">
+      <c r="E114" s="29">
+        <v>0</v>
+      </c>
+      <c r="F114" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G114" s="29">
+      <c r="G114" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4664,14 +4675,14 @@
       </c>
       <c r="C115" s="12"/>
       <c r="D115" s="13"/>
-      <c r="E115" s="30">
-        <v>0</v>
-      </c>
-      <c r="F115" s="30">
+      <c r="E115" s="29">
+        <v>0</v>
+      </c>
+      <c r="F115" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G115" s="29">
+      <c r="G115" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4685,14 +4696,14 @@
       </c>
       <c r="C116" s="12"/>
       <c r="D116" s="13"/>
-      <c r="E116" s="30">
-        <v>0</v>
-      </c>
-      <c r="F116" s="30">
+      <c r="E116" s="29">
+        <v>0</v>
+      </c>
+      <c r="F116" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G116" s="29">
+      <c r="G116" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4706,14 +4717,14 @@
       </c>
       <c r="C117" s="12"/>
       <c r="D117" s="13"/>
-      <c r="E117" s="30">
-        <v>0</v>
-      </c>
-      <c r="F117" s="30">
+      <c r="E117" s="29">
+        <v>0</v>
+      </c>
+      <c r="F117" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G117" s="29">
+      <c r="G117" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4727,14 +4738,14 @@
       </c>
       <c r="C118" s="12"/>
       <c r="D118" s="13"/>
-      <c r="E118" s="30">
-        <v>0</v>
-      </c>
-      <c r="F118" s="30">
+      <c r="E118" s="29">
+        <v>0</v>
+      </c>
+      <c r="F118" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G118" s="29">
+      <c r="G118" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4748,14 +4759,14 @@
       </c>
       <c r="C119" s="12"/>
       <c r="D119" s="13"/>
-      <c r="E119" s="30">
-        <v>0</v>
-      </c>
-      <c r="F119" s="30">
+      <c r="E119" s="29">
+        <v>0</v>
+      </c>
+      <c r="F119" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G119" s="29">
+      <c r="G119" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4769,14 +4780,14 @@
       </c>
       <c r="C120" s="12"/>
       <c r="D120" s="13"/>
-      <c r="E120" s="30">
-        <v>0</v>
-      </c>
-      <c r="F120" s="30">
+      <c r="E120" s="29">
+        <v>0</v>
+      </c>
+      <c r="F120" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G120" s="29">
+      <c r="G120" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4790,14 +4801,14 @@
       </c>
       <c r="C121" s="12"/>
       <c r="D121" s="13"/>
-      <c r="E121" s="30">
-        <v>0</v>
-      </c>
-      <c r="F121" s="30">
+      <c r="E121" s="29">
+        <v>0</v>
+      </c>
+      <c r="F121" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G121" s="29">
+      <c r="G121" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4811,14 +4822,14 @@
       </c>
       <c r="C122" s="12"/>
       <c r="D122" s="13"/>
-      <c r="E122" s="30">
-        <v>0</v>
-      </c>
-      <c r="F122" s="30">
+      <c r="E122" s="29">
+        <v>0</v>
+      </c>
+      <c r="F122" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G122" s="29">
+      <c r="G122" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4832,14 +4843,14 @@
       </c>
       <c r="C123" s="12"/>
       <c r="D123" s="13"/>
-      <c r="E123" s="30">
-        <v>0</v>
-      </c>
-      <c r="F123" s="30">
+      <c r="E123" s="29">
+        <v>0</v>
+      </c>
+      <c r="F123" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G123" s="29">
+      <c r="G123" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4853,14 +4864,14 @@
       </c>
       <c r="C124" s="12"/>
       <c r="D124" s="13"/>
-      <c r="E124" s="30">
-        <v>0</v>
-      </c>
-      <c r="F124" s="30">
+      <c r="E124" s="29">
+        <v>0</v>
+      </c>
+      <c r="F124" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G124" s="29">
+      <c r="G124" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4874,14 +4885,14 @@
       </c>
       <c r="C125" s="12"/>
       <c r="D125" s="13"/>
-      <c r="E125" s="30">
-        <v>0</v>
-      </c>
-      <c r="F125" s="30">
+      <c r="E125" s="29">
+        <v>0</v>
+      </c>
+      <c r="F125" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G125" s="29">
+      <c r="G125" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4895,14 +4906,14 @@
       </c>
       <c r="C126" s="12"/>
       <c r="D126" s="13"/>
-      <c r="E126" s="30">
-        <v>0</v>
-      </c>
-      <c r="F126" s="30">
+      <c r="E126" s="29">
+        <v>0</v>
+      </c>
+      <c r="F126" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G126" s="29">
+      <c r="G126" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4916,14 +4927,14 @@
       </c>
       <c r="C127" s="12"/>
       <c r="D127" s="13"/>
-      <c r="E127" s="30">
-        <v>0</v>
-      </c>
-      <c r="F127" s="30">
+      <c r="E127" s="29">
+        <v>0</v>
+      </c>
+      <c r="F127" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G127" s="29">
+      <c r="G127" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4937,14 +4948,14 @@
       </c>
       <c r="C128" s="12"/>
       <c r="D128" s="13"/>
-      <c r="E128" s="30">
-        <v>0</v>
-      </c>
-      <c r="F128" s="30">
+      <c r="E128" s="29">
+        <v>0</v>
+      </c>
+      <c r="F128" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G128" s="29">
+      <c r="G128" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4958,14 +4969,14 @@
       </c>
       <c r="C129" s="12"/>
       <c r="D129" s="13"/>
-      <c r="E129" s="30">
-        <v>0</v>
-      </c>
-      <c r="F129" s="30">
+      <c r="E129" s="29">
+        <v>0</v>
+      </c>
+      <c r="F129" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G129" s="29">
+      <c r="G129" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4979,14 +4990,14 @@
       </c>
       <c r="C130" s="12"/>
       <c r="D130" s="13"/>
-      <c r="E130" s="30">
-        <v>0</v>
-      </c>
-      <c r="F130" s="30">
+      <c r="E130" s="29">
+        <v>0</v>
+      </c>
+      <c r="F130" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G130" s="29">
+      <c r="G130" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5000,14 +5011,14 @@
       </c>
       <c r="C131" s="12"/>
       <c r="D131" s="13"/>
-      <c r="E131" s="30">
-        <v>0</v>
-      </c>
-      <c r="F131" s="30">
+      <c r="E131" s="29">
+        <v>0</v>
+      </c>
+      <c r="F131" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G131" s="29">
+      <c r="G131" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5021,14 +5032,14 @@
       </c>
       <c r="C132" s="12"/>
       <c r="D132" s="13"/>
-      <c r="E132" s="30">
-        <v>0</v>
-      </c>
-      <c r="F132" s="30">
+      <c r="E132" s="29">
+        <v>0</v>
+      </c>
+      <c r="F132" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G132" s="29">
+      <c r="G132" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5042,14 +5053,14 @@
       </c>
       <c r="C133" s="12"/>
       <c r="D133" s="13"/>
-      <c r="E133" s="30">
-        <v>0</v>
-      </c>
-      <c r="F133" s="30">
+      <c r="E133" s="29">
+        <v>0</v>
+      </c>
+      <c r="F133" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G133" s="29">
+      <c r="G133" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5063,14 +5074,14 @@
       </c>
       <c r="C134" s="12"/>
       <c r="D134" s="13"/>
-      <c r="E134" s="30">
-        <v>0</v>
-      </c>
-      <c r="F134" s="30">
+      <c r="E134" s="29">
+        <v>0</v>
+      </c>
+      <c r="F134" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G134" s="29">
+      <c r="G134" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5084,14 +5095,14 @@
       </c>
       <c r="C135" s="12"/>
       <c r="D135" s="13"/>
-      <c r="E135" s="30">
-        <v>0</v>
-      </c>
-      <c r="F135" s="30">
+      <c r="E135" s="29">
+        <v>0</v>
+      </c>
+      <c r="F135" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G135" s="29">
+      <c r="G135" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5105,14 +5116,14 @@
       </c>
       <c r="C136" s="12"/>
       <c r="D136" s="13"/>
-      <c r="E136" s="30">
-        <v>0</v>
-      </c>
-      <c r="F136" s="30">
+      <c r="E136" s="29">
+        <v>0</v>
+      </c>
+      <c r="F136" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G136" s="29">
+      <c r="G136" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5126,14 +5137,14 @@
       </c>
       <c r="C137" s="12"/>
       <c r="D137" s="13"/>
-      <c r="E137" s="30">
-        <v>0</v>
-      </c>
-      <c r="F137" s="30">
+      <c r="E137" s="29">
+        <v>0</v>
+      </c>
+      <c r="F137" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G137" s="29">
+      <c r="G137" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5147,14 +5158,14 @@
       </c>
       <c r="C138" s="12"/>
       <c r="D138" s="13"/>
-      <c r="E138" s="30">
-        <v>0</v>
-      </c>
-      <c r="F138" s="30">
+      <c r="E138" s="29">
+        <v>0</v>
+      </c>
+      <c r="F138" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G138" s="29">
+      <c r="G138" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5168,14 +5179,14 @@
       </c>
       <c r="C139" s="12"/>
       <c r="D139" s="13"/>
-      <c r="E139" s="30">
-        <v>0</v>
-      </c>
-      <c r="F139" s="30">
+      <c r="E139" s="29">
+        <v>0</v>
+      </c>
+      <c r="F139" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G139" s="29">
+      <c r="G139" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5189,14 +5200,14 @@
       </c>
       <c r="C140" s="12"/>
       <c r="D140" s="13"/>
-      <c r="E140" s="30">
-        <v>0</v>
-      </c>
-      <c r="F140" s="30">
+      <c r="E140" s="29">
+        <v>0</v>
+      </c>
+      <c r="F140" s="29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G140" s="29">
+      <c r="G140" s="28">
         <f t="shared" ref="G140:G203" si="12">HOUR($D140-$C140)+MINUTE($D140-$C140)/60</f>
         <v>0</v>
       </c>
@@ -5210,14 +5221,14 @@
       </c>
       <c r="C141" s="12"/>
       <c r="D141" s="13"/>
-      <c r="E141" s="30">
-        <v>0</v>
-      </c>
-      <c r="F141" s="30">
+      <c r="E141" s="29">
+        <v>0</v>
+      </c>
+      <c r="F141" s="29">
         <f t="shared" ref="F141:F204" si="13">G141-E141</f>
         <v>0</v>
       </c>
-      <c r="G141" s="29">
+      <c r="G141" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5231,14 +5242,14 @@
       </c>
       <c r="C142" s="12"/>
       <c r="D142" s="13"/>
-      <c r="E142" s="30">
-        <v>0</v>
-      </c>
-      <c r="F142" s="30">
+      <c r="E142" s="29">
+        <v>0</v>
+      </c>
+      <c r="F142" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G142" s="29">
+      <c r="G142" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5252,14 +5263,14 @@
       </c>
       <c r="C143" s="12"/>
       <c r="D143" s="13"/>
-      <c r="E143" s="30">
-        <v>0</v>
-      </c>
-      <c r="F143" s="30">
+      <c r="E143" s="29">
+        <v>0</v>
+      </c>
+      <c r="F143" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G143" s="29">
+      <c r="G143" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5273,14 +5284,14 @@
       </c>
       <c r="C144" s="12"/>
       <c r="D144" s="13"/>
-      <c r="E144" s="30">
-        <v>0</v>
-      </c>
-      <c r="F144" s="30">
+      <c r="E144" s="29">
+        <v>0</v>
+      </c>
+      <c r="F144" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G144" s="29">
+      <c r="G144" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5294,14 +5305,14 @@
       </c>
       <c r="C145" s="12"/>
       <c r="D145" s="13"/>
-      <c r="E145" s="30">
-        <v>0</v>
-      </c>
-      <c r="F145" s="30">
+      <c r="E145" s="29">
+        <v>0</v>
+      </c>
+      <c r="F145" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G145" s="29">
+      <c r="G145" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5315,14 +5326,14 @@
       </c>
       <c r="C146" s="12"/>
       <c r="D146" s="13"/>
-      <c r="E146" s="30">
-        <v>0</v>
-      </c>
-      <c r="F146" s="30">
+      <c r="E146" s="29">
+        <v>0</v>
+      </c>
+      <c r="F146" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G146" s="29">
+      <c r="G146" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5336,14 +5347,14 @@
       </c>
       <c r="C147" s="12"/>
       <c r="D147" s="13"/>
-      <c r="E147" s="30">
-        <v>0</v>
-      </c>
-      <c r="F147" s="30">
+      <c r="E147" s="29">
+        <v>0</v>
+      </c>
+      <c r="F147" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G147" s="29">
+      <c r="G147" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5357,14 +5368,14 @@
       </c>
       <c r="C148" s="12"/>
       <c r="D148" s="13"/>
-      <c r="E148" s="30">
-        <v>0</v>
-      </c>
-      <c r="F148" s="30">
+      <c r="E148" s="29">
+        <v>0</v>
+      </c>
+      <c r="F148" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G148" s="29">
+      <c r="G148" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5378,14 +5389,14 @@
       </c>
       <c r="C149" s="12"/>
       <c r="D149" s="13"/>
-      <c r="E149" s="30">
-        <v>0</v>
-      </c>
-      <c r="F149" s="30">
+      <c r="E149" s="29">
+        <v>0</v>
+      </c>
+      <c r="F149" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G149" s="29">
+      <c r="G149" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5399,14 +5410,14 @@
       </c>
       <c r="C150" s="12"/>
       <c r="D150" s="13"/>
-      <c r="E150" s="30">
-        <v>0</v>
-      </c>
-      <c r="F150" s="30">
+      <c r="E150" s="29">
+        <v>0</v>
+      </c>
+      <c r="F150" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G150" s="29">
+      <c r="G150" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5420,14 +5431,14 @@
       </c>
       <c r="C151" s="12"/>
       <c r="D151" s="13"/>
-      <c r="E151" s="30">
-        <v>0</v>
-      </c>
-      <c r="F151" s="30">
+      <c r="E151" s="29">
+        <v>0</v>
+      </c>
+      <c r="F151" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G151" s="29">
+      <c r="G151" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5441,14 +5452,14 @@
       </c>
       <c r="C152" s="12"/>
       <c r="D152" s="13"/>
-      <c r="E152" s="30">
-        <v>0</v>
-      </c>
-      <c r="F152" s="30">
+      <c r="E152" s="29">
+        <v>0</v>
+      </c>
+      <c r="F152" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G152" s="29">
+      <c r="G152" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5462,14 +5473,14 @@
       </c>
       <c r="C153" s="12"/>
       <c r="D153" s="13"/>
-      <c r="E153" s="30">
-        <v>0</v>
-      </c>
-      <c r="F153" s="30">
+      <c r="E153" s="29">
+        <v>0</v>
+      </c>
+      <c r="F153" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G153" s="29">
+      <c r="G153" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5483,14 +5494,14 @@
       </c>
       <c r="C154" s="12"/>
       <c r="D154" s="13"/>
-      <c r="E154" s="30">
-        <v>0</v>
-      </c>
-      <c r="F154" s="30">
+      <c r="E154" s="29">
+        <v>0</v>
+      </c>
+      <c r="F154" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G154" s="29">
+      <c r="G154" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5504,14 +5515,14 @@
       </c>
       <c r="C155" s="12"/>
       <c r="D155" s="13"/>
-      <c r="E155" s="30">
-        <v>0</v>
-      </c>
-      <c r="F155" s="30">
+      <c r="E155" s="29">
+        <v>0</v>
+      </c>
+      <c r="F155" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G155" s="29">
+      <c r="G155" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5525,14 +5536,14 @@
       </c>
       <c r="C156" s="12"/>
       <c r="D156" s="13"/>
-      <c r="E156" s="30">
-        <v>0</v>
-      </c>
-      <c r="F156" s="30">
+      <c r="E156" s="29">
+        <v>0</v>
+      </c>
+      <c r="F156" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G156" s="29">
+      <c r="G156" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5546,14 +5557,14 @@
       </c>
       <c r="C157" s="12"/>
       <c r="D157" s="13"/>
-      <c r="E157" s="30">
-        <v>0</v>
-      </c>
-      <c r="F157" s="30">
+      <c r="E157" s="29">
+        <v>0</v>
+      </c>
+      <c r="F157" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G157" s="29">
+      <c r="G157" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5567,14 +5578,14 @@
       </c>
       <c r="C158" s="12"/>
       <c r="D158" s="13"/>
-      <c r="E158" s="30">
-        <v>0</v>
-      </c>
-      <c r="F158" s="30">
+      <c r="E158" s="29">
+        <v>0</v>
+      </c>
+      <c r="F158" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G158" s="29">
+      <c r="G158" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5588,14 +5599,14 @@
       </c>
       <c r="C159" s="12"/>
       <c r="D159" s="13"/>
-      <c r="E159" s="30">
-        <v>0</v>
-      </c>
-      <c r="F159" s="30">
+      <c r="E159" s="29">
+        <v>0</v>
+      </c>
+      <c r="F159" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G159" s="29">
+      <c r="G159" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5609,14 +5620,14 @@
       </c>
       <c r="C160" s="12"/>
       <c r="D160" s="13"/>
-      <c r="E160" s="30">
-        <v>0</v>
-      </c>
-      <c r="F160" s="30">
+      <c r="E160" s="29">
+        <v>0</v>
+      </c>
+      <c r="F160" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G160" s="29">
+      <c r="G160" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5630,14 +5641,14 @@
       </c>
       <c r="C161" s="12"/>
       <c r="D161" s="13"/>
-      <c r="E161" s="30">
-        <v>0</v>
-      </c>
-      <c r="F161" s="30">
+      <c r="E161" s="29">
+        <v>0</v>
+      </c>
+      <c r="F161" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G161" s="29">
+      <c r="G161" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5651,14 +5662,14 @@
       </c>
       <c r="C162" s="12"/>
       <c r="D162" s="13"/>
-      <c r="E162" s="30">
-        <v>0</v>
-      </c>
-      <c r="F162" s="30">
+      <c r="E162" s="29">
+        <v>0</v>
+      </c>
+      <c r="F162" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G162" s="29">
+      <c r="G162" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5672,14 +5683,14 @@
       </c>
       <c r="C163" s="12"/>
       <c r="D163" s="13"/>
-      <c r="E163" s="30">
-        <v>0</v>
-      </c>
-      <c r="F163" s="30">
+      <c r="E163" s="29">
+        <v>0</v>
+      </c>
+      <c r="F163" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G163" s="29">
+      <c r="G163" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5693,14 +5704,14 @@
       </c>
       <c r="C164" s="12"/>
       <c r="D164" s="13"/>
-      <c r="E164" s="30">
-        <v>0</v>
-      </c>
-      <c r="F164" s="30">
+      <c r="E164" s="29">
+        <v>0</v>
+      </c>
+      <c r="F164" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G164" s="29">
+      <c r="G164" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5714,14 +5725,14 @@
       </c>
       <c r="C165" s="12"/>
       <c r="D165" s="13"/>
-      <c r="E165" s="30">
-        <v>0</v>
-      </c>
-      <c r="F165" s="30">
+      <c r="E165" s="29">
+        <v>0</v>
+      </c>
+      <c r="F165" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G165" s="29">
+      <c r="G165" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5735,14 +5746,14 @@
       </c>
       <c r="C166" s="12"/>
       <c r="D166" s="13"/>
-      <c r="E166" s="30">
-        <v>0</v>
-      </c>
-      <c r="F166" s="30">
+      <c r="E166" s="29">
+        <v>0</v>
+      </c>
+      <c r="F166" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G166" s="29">
+      <c r="G166" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5756,14 +5767,14 @@
       </c>
       <c r="C167" s="12"/>
       <c r="D167" s="13"/>
-      <c r="E167" s="30">
-        <v>0</v>
-      </c>
-      <c r="F167" s="30">
+      <c r="E167" s="29">
+        <v>0</v>
+      </c>
+      <c r="F167" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G167" s="29">
+      <c r="G167" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5777,14 +5788,14 @@
       </c>
       <c r="C168" s="12"/>
       <c r="D168" s="13"/>
-      <c r="E168" s="30">
-        <v>0</v>
-      </c>
-      <c r="F168" s="30">
+      <c r="E168" s="29">
+        <v>0</v>
+      </c>
+      <c r="F168" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G168" s="29">
+      <c r="G168" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5798,14 +5809,14 @@
       </c>
       <c r="C169" s="12"/>
       <c r="D169" s="13"/>
-      <c r="E169" s="30">
-        <v>0</v>
-      </c>
-      <c r="F169" s="30">
+      <c r="E169" s="29">
+        <v>0</v>
+      </c>
+      <c r="F169" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G169" s="29">
+      <c r="G169" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5819,14 +5830,14 @@
       </c>
       <c r="C170" s="12"/>
       <c r="D170" s="13"/>
-      <c r="E170" s="30">
-        <v>0</v>
-      </c>
-      <c r="F170" s="30">
+      <c r="E170" s="29">
+        <v>0</v>
+      </c>
+      <c r="F170" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G170" s="29">
+      <c r="G170" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5840,14 +5851,14 @@
       </c>
       <c r="C171" s="12"/>
       <c r="D171" s="13"/>
-      <c r="E171" s="30">
-        <v>0</v>
-      </c>
-      <c r="F171" s="30">
+      <c r="E171" s="29">
+        <v>0</v>
+      </c>
+      <c r="F171" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G171" s="29">
+      <c r="G171" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5861,14 +5872,14 @@
       </c>
       <c r="C172" s="12"/>
       <c r="D172" s="13"/>
-      <c r="E172" s="30">
-        <v>0</v>
-      </c>
-      <c r="F172" s="30">
+      <c r="E172" s="29">
+        <v>0</v>
+      </c>
+      <c r="F172" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G172" s="29">
+      <c r="G172" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5882,14 +5893,14 @@
       </c>
       <c r="C173" s="12"/>
       <c r="D173" s="13"/>
-      <c r="E173" s="30">
-        <v>0</v>
-      </c>
-      <c r="F173" s="30">
+      <c r="E173" s="29">
+        <v>0</v>
+      </c>
+      <c r="F173" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G173" s="29">
+      <c r="G173" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5903,14 +5914,14 @@
       </c>
       <c r="C174" s="12"/>
       <c r="D174" s="13"/>
-      <c r="E174" s="30">
-        <v>0</v>
-      </c>
-      <c r="F174" s="30">
+      <c r="E174" s="29">
+        <v>0</v>
+      </c>
+      <c r="F174" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G174" s="29">
+      <c r="G174" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5924,14 +5935,14 @@
       </c>
       <c r="C175" s="12"/>
       <c r="D175" s="13"/>
-      <c r="E175" s="30">
-        <v>0</v>
-      </c>
-      <c r="F175" s="30">
+      <c r="E175" s="29">
+        <v>0</v>
+      </c>
+      <c r="F175" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G175" s="29">
+      <c r="G175" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5945,14 +5956,14 @@
       </c>
       <c r="C176" s="12"/>
       <c r="D176" s="13"/>
-      <c r="E176" s="30">
-        <v>0</v>
-      </c>
-      <c r="F176" s="30">
+      <c r="E176" s="29">
+        <v>0</v>
+      </c>
+      <c r="F176" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G176" s="29">
+      <c r="G176" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5966,14 +5977,14 @@
       </c>
       <c r="C177" s="12"/>
       <c r="D177" s="13"/>
-      <c r="E177" s="30">
-        <v>0</v>
-      </c>
-      <c r="F177" s="30">
+      <c r="E177" s="29">
+        <v>0</v>
+      </c>
+      <c r="F177" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G177" s="29">
+      <c r="G177" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5987,14 +5998,14 @@
       </c>
       <c r="C178" s="12"/>
       <c r="D178" s="13"/>
-      <c r="E178" s="30">
-        <v>0</v>
-      </c>
-      <c r="F178" s="30">
+      <c r="E178" s="29">
+        <v>0</v>
+      </c>
+      <c r="F178" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G178" s="29">
+      <c r="G178" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6008,14 +6019,14 @@
       </c>
       <c r="C179" s="12"/>
       <c r="D179" s="13"/>
-      <c r="E179" s="30">
-        <v>0</v>
-      </c>
-      <c r="F179" s="30">
+      <c r="E179" s="29">
+        <v>0</v>
+      </c>
+      <c r="F179" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G179" s="29">
+      <c r="G179" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6029,14 +6040,14 @@
       </c>
       <c r="C180" s="12"/>
       <c r="D180" s="13"/>
-      <c r="E180" s="30">
-        <v>0</v>
-      </c>
-      <c r="F180" s="30">
+      <c r="E180" s="29">
+        <v>0</v>
+      </c>
+      <c r="F180" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G180" s="29">
+      <c r="G180" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6050,14 +6061,14 @@
       </c>
       <c r="C181" s="12"/>
       <c r="D181" s="13"/>
-      <c r="E181" s="30">
-        <v>0</v>
-      </c>
-      <c r="F181" s="30">
+      <c r="E181" s="29">
+        <v>0</v>
+      </c>
+      <c r="F181" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G181" s="29">
+      <c r="G181" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6071,14 +6082,14 @@
       </c>
       <c r="C182" s="12"/>
       <c r="D182" s="13"/>
-      <c r="E182" s="30">
-        <v>0</v>
-      </c>
-      <c r="F182" s="30">
+      <c r="E182" s="29">
+        <v>0</v>
+      </c>
+      <c r="F182" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G182" s="29">
+      <c r="G182" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6092,14 +6103,14 @@
       </c>
       <c r="C183" s="12"/>
       <c r="D183" s="13"/>
-      <c r="E183" s="30">
-        <v>0</v>
-      </c>
-      <c r="F183" s="30">
+      <c r="E183" s="29">
+        <v>0</v>
+      </c>
+      <c r="F183" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G183" s="29">
+      <c r="G183" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6113,14 +6124,14 @@
       </c>
       <c r="C184" s="12"/>
       <c r="D184" s="13"/>
-      <c r="E184" s="30">
-        <v>0</v>
-      </c>
-      <c r="F184" s="30">
+      <c r="E184" s="29">
+        <v>0</v>
+      </c>
+      <c r="F184" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G184" s="29">
+      <c r="G184" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6134,14 +6145,14 @@
       </c>
       <c r="C185" s="12"/>
       <c r="D185" s="13"/>
-      <c r="E185" s="30">
-        <v>0</v>
-      </c>
-      <c r="F185" s="30">
+      <c r="E185" s="29">
+        <v>0</v>
+      </c>
+      <c r="F185" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G185" s="29">
+      <c r="G185" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6155,14 +6166,14 @@
       </c>
       <c r="C186" s="12"/>
       <c r="D186" s="13"/>
-      <c r="E186" s="30">
-        <v>0</v>
-      </c>
-      <c r="F186" s="30">
+      <c r="E186" s="29">
+        <v>0</v>
+      </c>
+      <c r="F186" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G186" s="29">
+      <c r="G186" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6176,14 +6187,14 @@
       </c>
       <c r="C187" s="12"/>
       <c r="D187" s="13"/>
-      <c r="E187" s="30">
-        <v>0</v>
-      </c>
-      <c r="F187" s="30">
+      <c r="E187" s="29">
+        <v>0</v>
+      </c>
+      <c r="F187" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G187" s="29">
+      <c r="G187" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6197,14 +6208,14 @@
       </c>
       <c r="C188" s="12"/>
       <c r="D188" s="13"/>
-      <c r="E188" s="30">
-        <v>0</v>
-      </c>
-      <c r="F188" s="30">
+      <c r="E188" s="29">
+        <v>0</v>
+      </c>
+      <c r="F188" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G188" s="29">
+      <c r="G188" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6218,14 +6229,14 @@
       </c>
       <c r="C189" s="12"/>
       <c r="D189" s="13"/>
-      <c r="E189" s="30">
-        <v>0</v>
-      </c>
-      <c r="F189" s="30">
+      <c r="E189" s="29">
+        <v>0</v>
+      </c>
+      <c r="F189" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G189" s="29">
+      <c r="G189" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6239,14 +6250,14 @@
       </c>
       <c r="C190" s="12"/>
       <c r="D190" s="13"/>
-      <c r="E190" s="30">
-        <v>0</v>
-      </c>
-      <c r="F190" s="30">
+      <c r="E190" s="29">
+        <v>0</v>
+      </c>
+      <c r="F190" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G190" s="29">
+      <c r="G190" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6260,14 +6271,14 @@
       </c>
       <c r="C191" s="12"/>
       <c r="D191" s="13"/>
-      <c r="E191" s="30">
-        <v>0</v>
-      </c>
-      <c r="F191" s="30">
+      <c r="E191" s="29">
+        <v>0</v>
+      </c>
+      <c r="F191" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G191" s="29">
+      <c r="G191" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6281,14 +6292,14 @@
       </c>
       <c r="C192" s="12"/>
       <c r="D192" s="13"/>
-      <c r="E192" s="30">
-        <v>0</v>
-      </c>
-      <c r="F192" s="30">
+      <c r="E192" s="29">
+        <v>0</v>
+      </c>
+      <c r="F192" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G192" s="29">
+      <c r="G192" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6302,14 +6313,14 @@
       </c>
       <c r="C193" s="12"/>
       <c r="D193" s="13"/>
-      <c r="E193" s="30">
-        <v>0</v>
-      </c>
-      <c r="F193" s="30">
+      <c r="E193" s="29">
+        <v>0</v>
+      </c>
+      <c r="F193" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G193" s="29">
+      <c r="G193" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6323,14 +6334,14 @@
       </c>
       <c r="C194" s="12"/>
       <c r="D194" s="13"/>
-      <c r="E194" s="30">
-        <v>0</v>
-      </c>
-      <c r="F194" s="30">
+      <c r="E194" s="29">
+        <v>0</v>
+      </c>
+      <c r="F194" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G194" s="29">
+      <c r="G194" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6344,14 +6355,14 @@
       </c>
       <c r="C195" s="12"/>
       <c r="D195" s="13"/>
-      <c r="E195" s="30">
-        <v>0</v>
-      </c>
-      <c r="F195" s="30">
+      <c r="E195" s="29">
+        <v>0</v>
+      </c>
+      <c r="F195" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G195" s="29">
+      <c r="G195" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6365,14 +6376,14 @@
       </c>
       <c r="C196" s="12"/>
       <c r="D196" s="13"/>
-      <c r="E196" s="30">
-        <v>0</v>
-      </c>
-      <c r="F196" s="30">
+      <c r="E196" s="29">
+        <v>0</v>
+      </c>
+      <c r="F196" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G196" s="29">
+      <c r="G196" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6386,14 +6397,14 @@
       </c>
       <c r="C197" s="12"/>
       <c r="D197" s="13"/>
-      <c r="E197" s="30">
-        <v>0</v>
-      </c>
-      <c r="F197" s="30">
+      <c r="E197" s="29">
+        <v>0</v>
+      </c>
+      <c r="F197" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G197" s="29">
+      <c r="G197" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6407,14 +6418,14 @@
       </c>
       <c r="C198" s="12"/>
       <c r="D198" s="13"/>
-      <c r="E198" s="30">
-        <v>0</v>
-      </c>
-      <c r="F198" s="30">
+      <c r="E198" s="29">
+        <v>0</v>
+      </c>
+      <c r="F198" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G198" s="29">
+      <c r="G198" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6428,14 +6439,14 @@
       </c>
       <c r="C199" s="12"/>
       <c r="D199" s="13"/>
-      <c r="E199" s="30">
-        <v>0</v>
-      </c>
-      <c r="F199" s="30">
+      <c r="E199" s="29">
+        <v>0</v>
+      </c>
+      <c r="F199" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G199" s="29">
+      <c r="G199" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6449,14 +6460,14 @@
       </c>
       <c r="C200" s="12"/>
       <c r="D200" s="13"/>
-      <c r="E200" s="30">
-        <v>0</v>
-      </c>
-      <c r="F200" s="30">
+      <c r="E200" s="29">
+        <v>0</v>
+      </c>
+      <c r="F200" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G200" s="29">
+      <c r="G200" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6470,14 +6481,14 @@
       </c>
       <c r="C201" s="12"/>
       <c r="D201" s="13"/>
-      <c r="E201" s="30">
-        <v>0</v>
-      </c>
-      <c r="F201" s="30">
+      <c r="E201" s="29">
+        <v>0</v>
+      </c>
+      <c r="F201" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G201" s="29">
+      <c r="G201" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6491,14 +6502,14 @@
       </c>
       <c r="C202" s="12"/>
       <c r="D202" s="13"/>
-      <c r="E202" s="30">
-        <v>0</v>
-      </c>
-      <c r="F202" s="30">
+      <c r="E202" s="29">
+        <v>0</v>
+      </c>
+      <c r="F202" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G202" s="29">
+      <c r="G202" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6512,14 +6523,14 @@
       </c>
       <c r="C203" s="12"/>
       <c r="D203" s="13"/>
-      <c r="E203" s="30">
-        <v>0</v>
-      </c>
-      <c r="F203" s="30">
+      <c r="E203" s="29">
+        <v>0</v>
+      </c>
+      <c r="F203" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G203" s="29">
+      <c r="G203" s="28">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -6533,14 +6544,14 @@
       </c>
       <c r="C204" s="12"/>
       <c r="D204" s="13"/>
-      <c r="E204" s="30">
-        <v>0</v>
-      </c>
-      <c r="F204" s="30">
+      <c r="E204" s="29">
+        <v>0</v>
+      </c>
+      <c r="F204" s="29">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G204" s="29">
+      <c r="G204" s="28">
         <f t="shared" ref="G204:G209" si="15">HOUR($D204-$C204)+MINUTE($D204-$C204)/60</f>
         <v>0</v>
       </c>
@@ -6554,14 +6565,14 @@
       </c>
       <c r="C205" s="12"/>
       <c r="D205" s="13"/>
-      <c r="E205" s="30">
-        <v>0</v>
-      </c>
-      <c r="F205" s="30">
+      <c r="E205" s="29">
+        <v>0</v>
+      </c>
+      <c r="F205" s="29">
         <f t="shared" ref="F205:F209" si="16">G205-E205</f>
         <v>0</v>
       </c>
-      <c r="G205" s="29">
+      <c r="G205" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6575,14 +6586,14 @@
       </c>
       <c r="C206" s="12"/>
       <c r="D206" s="13"/>
-      <c r="E206" s="30">
-        <v>0</v>
-      </c>
-      <c r="F206" s="30">
+      <c r="E206" s="29">
+        <v>0</v>
+      </c>
+      <c r="F206" s="29">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G206" s="29">
+      <c r="G206" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6596,14 +6607,14 @@
       </c>
       <c r="C207" s="12"/>
       <c r="D207" s="13"/>
-      <c r="E207" s="30">
-        <v>0</v>
-      </c>
-      <c r="F207" s="30">
+      <c r="E207" s="29">
+        <v>0</v>
+      </c>
+      <c r="F207" s="29">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G207" s="29">
+      <c r="G207" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6617,14 +6628,14 @@
       </c>
       <c r="C208" s="12"/>
       <c r="D208" s="13"/>
-      <c r="E208" s="30">
-        <v>0</v>
-      </c>
-      <c r="F208" s="30">
+      <c r="E208" s="29">
+        <v>0</v>
+      </c>
+      <c r="F208" s="29">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G208" s="29">
+      <c r="G208" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6638,14 +6649,14 @@
       </c>
       <c r="C209" s="19"/>
       <c r="D209" s="20"/>
-      <c r="E209" s="30">
-        <v>0</v>
-      </c>
-      <c r="F209" s="30">
+      <c r="E209" s="29">
+        <v>0</v>
+      </c>
+      <c r="F209" s="29">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G209" s="29">
+      <c r="G209" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6693,16 +6704,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6711,29 +6722,29 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -6742,135 +6753,135 @@
     </row>
     <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="34">
+      <c r="A7" s="33">
         <v>42900</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>80</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <v>75</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="35">
         <v>70</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="38"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="38"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="38"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="38"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="38"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="54"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6902,13 +6913,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>6.6666666666666661</v>
+        <v>10.083333333333332</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
@@ -6943,7 +6954,7 @@
       </c>
       <c r="D13" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$58,Wochenstunden!$C13,Begleitprotokoll!$G$5:$G$58)</f>
-        <v>0</v>
+        <v>3.4166666666666665</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
@@ -7408,15 +7419,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FDFE56A80EF5442A8C49F1A53575DCB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="779f73c3c36cf7ba200988a4ca77eaef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59fe8e26-cc10-4df5-9438-4b376e72b413" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0236c16f4b075c0c7c9c75a395e36d7f" ns2:_="">
     <xsd:import namespace="59fe8e26-cc10-4df5-9438-4b376e72b413"/>
@@ -7560,21 +7562,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2DD5AC-C113-4029-AC2A-CE7CE7D85D8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7592,7 +7595,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -7605,4 +7608,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Vault backup: 22/05/24 16:28:56 XMG-MAZ SHUTDOWN
</commit_message>
<xml_diff>
--- a/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
+++ b/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\2023_24_4BHITS\A_Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C691244-39D6-40BB-A150-0A75667387F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45DB245-4901-413B-B0C0-CA94643FE0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Begleitprotokoll" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Name:</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Matthias Hrbek</t>
+  </si>
+  <si>
+    <t>Okto TV Workshop</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1260,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2000,7 +2003,7 @@
   <dimension ref="A1:HZ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2038,15 +2041,15 @@
       <c r="D2" s="44"/>
       <c r="E2" s="24">
         <f>SUM(E5:E209)</f>
-        <v>4.25</v>
+        <v>8.629999999999999</v>
       </c>
       <c r="F2" s="24">
         <f>SUM(F5:F209)</f>
-        <v>5.8333333333333321</v>
+        <v>8.0366666666666653</v>
       </c>
       <c r="G2" s="25">
         <f>SUM(G5:G209)</f>
-        <v>10.083333333333332</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="H2" s="26"/>
     </row>
@@ -2463,25 +2466,33 @@
       </c>
     </row>
     <row r="10" spans="1:234" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="11" t="e">
+      <c r="A10" s="15">
+        <v>45433</v>
+      </c>
+      <c r="B10" s="11">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.63888888888888884</v>
+      </c>
       <c r="E10" s="29">
-        <v>0</v>
+        <v>4.38</v>
       </c>
       <c r="F10" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.2033333333333331</v>
       </c>
       <c r="G10" s="28">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="16"/>
+        <v>6.583333333333333</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
@@ -6919,7 +6930,7 @@
       <c r="D8" s="61"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>10.083333333333332</v>
+        <v>16.666666666666664</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
@@ -6981,7 +6992,7 @@
       </c>
       <c r="D16" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$58,Wochenstunden!$C16,Begleitprotokoll!$G$5:$G$58)</f>
-        <v>0</v>
+        <v>6.583333333333333</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
@@ -7419,6 +7430,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FDFE56A80EF5442A8C49F1A53575DCB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="779f73c3c36cf7ba200988a4ca77eaef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59fe8e26-cc10-4df5-9438-4b376e72b413" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0236c16f4b075c0c7c9c75a395e36d7f" ns2:_="">
     <xsd:import namespace="59fe8e26-cc10-4df5-9438-4b376e72b413"/>
@@ -7562,12 +7579,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7578,6 +7589,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2DD5AC-C113-4029-AC2A-CE7CE7D85D8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7595,21 +7621,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Vault backup: 23/05/24 16:18:11 XMG-MAZ SHUTDOWN
</commit_message>
<xml_diff>
--- a/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
+++ b/A_Diplomarbeit/DA_Zeitaufzeichnung_MEDT_Hrbek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\2023_24_4BHITS\A_Diplomarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45DB245-4901-413B-B0C0-CA94643FE0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699D8E2-5DD9-4DE5-8791-C3EF4DA7C7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Name:</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Okto TV Workshop</t>
+  </si>
+  <si>
+    <t>Testvideo/Audio analysiert und Verbesserungsvorschläge ausgearbeitet (mit Wissen von Okto)</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1263,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.583333333333333</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2003,7 +2006,7 @@
   <dimension ref="A1:HZ209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,11 +2048,11 @@
       </c>
       <c r="F2" s="24">
         <f>SUM(F5:F209)</f>
-        <v>8.0366666666666653</v>
+        <v>11.453333333333331</v>
       </c>
       <c r="G2" s="25">
         <f>SUM(G5:G209)</f>
-        <v>16.666666666666664</v>
+        <v>20.083333333333332</v>
       </c>
       <c r="H2" s="26"/>
     </row>
@@ -2495,25 +2498,33 @@
       </c>
     </row>
     <row r="11" spans="1:234" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="11" t="e">
+      <c r="A11" s="15">
+        <v>45435</v>
+      </c>
+      <c r="B11" s="11">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.69097222222222221</v>
+      </c>
       <c r="E11" s="29">
         <v>0</v>
       </c>
       <c r="F11" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.4166666666666665</v>
       </c>
       <c r="G11" s="28">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="16"/>
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:234" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
@@ -6917,7 +6928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C8:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="88" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
@@ -6930,7 +6941,7 @@
       <c r="D8" s="61"/>
       <c r="E8" s="1">
         <f>SUM(D11:D62)</f>
-        <v>16.666666666666664</v>
+        <v>20.083333333333332</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
@@ -6992,7 +7003,7 @@
       </c>
       <c r="D16" s="3">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$58,Wochenstunden!$C16,Begleitprotokoll!$G$5:$G$58)</f>
-        <v>6.583333333333333</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
@@ -7430,12 +7441,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FDFE56A80EF5442A8C49F1A53575DCB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="779f73c3c36cf7ba200988a4ca77eaef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59fe8e26-cc10-4df5-9438-4b376e72b413" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0236c16f4b075c0c7c9c75a395e36d7f" ns2:_="">
     <xsd:import namespace="59fe8e26-cc10-4df5-9438-4b376e72b413"/>
@@ -7579,6 +7584,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7589,21 +7600,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C2DD5AC-C113-4029-AC2A-CE7CE7D85D8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7621,6 +7617,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26077C71-CA3D-4DE3-BEC7-182FFBC9021C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5604A3-2520-4A5B-94D6-25D0FEB905F1}">
   <ds:schemaRefs>

</xml_diff>